<commit_message>
GameLevel.txt almost done reading in - crash bug on 4th line. Fix ASAP
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qsync\Graphics I &amp; II Shared Staff Folder\Project &amp; Portfolio IV\Week_3_Handout\Assignments\The Level Renderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421F74A-5ED2-4C97-92A8-617099FA0AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375CA647-A36F-44C4-AF30-47213B228907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="405" windowWidth="28305" windowHeight="16785" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="6255" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1415,6 +1415,9 @@
   </si>
   <si>
     <t>KEY FEATURES - 33% [unlocked by core, pick three]</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -2029,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2044,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -2128,8 +2131,11 @@
       <c r="C8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
upgraded project to lab 2 - H2B is working, not sure what all to take in from it yet.
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375CA647-A36F-44C4-AF30-47213B228907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09CCF55-D39B-47FE-A5B3-89D573661C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6255" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,6 +2087,9 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2402,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>15</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>28</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>16</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>34</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>17</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>18</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>27</v>
       </c>
@@ -2490,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>29</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>35</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>14</v>
       </c>
@@ -2523,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2546,7 +2549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>41</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>25</v>
       </c>
@@ -2567,8 +2570,11 @@
       <c r="C47" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Worked on project structured buffers, separated out shaders into .hlsl files
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09CCF55-D39B-47FE-A5B3-89D573661C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA8B41D-9A66-48BE-A6CF-6F16FEB282CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6255" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,6 +2065,9 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2075,6 +2078,9 @@
       </c>
       <c r="C3" s="3">
         <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Key Feature #1 (level swapping)
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9C0FF5-14CF-421F-8503-2B1AB2DB82D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C859059-19D0-458E-8137-B7AB1219A838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="4410" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,6 +2214,9 @@
       <c r="C14" s="3">
         <v>0</v>
       </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">

</xml_diff>

<commit_message>
new models for renderer
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C859059-19D0-458E-8137-B7AB1219A838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3482AF-799F-4D07-AFDD-B160B5066F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4410" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,6 +2121,9 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2132,6 +2135,9 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2157,6 +2163,9 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -2167,6 +2176,9 @@
       </c>
       <c r="C10" s="3">
         <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working parent / child relationship (shown in level 1)
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3482AF-799F-4D07-AFDD-B160B5066F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95626EBE-0DC1-41AA-A649-70B269D0EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
@@ -2273,8 +2273,11 @@
       <c r="C18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>30</v>
       </c>
@@ -2328,8 +2331,11 @@
       <c r="C23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>42</v>
       </c>
@@ -2340,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>19</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>12</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>20</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>13</v>
       </c>
@@ -2418,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Fixed Mini-map issues, finalized levels.
</commit_message>
<xml_diff>
--- a/utilities/Project Rubric.xlsx
+++ b/utilities/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Full Sail\Dev4\Week_3_Handout\Assignments\finalProject\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95626EBE-0DC1-41AA-A649-70B269D0EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CB951E-9287-403E-A8DD-872C6A68E277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="4410" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,6 +2589,9 @@
       <c r="C46" s="3">
         <v>0</v>
       </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">

</xml_diff>